<commit_message>
updated 0703data in the xlsx file
</commit_message>
<xml_diff>
--- a/data/lab1data.xlsx
+++ b/data/lab1data.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="50" windowWidth="19170" windowHeight="7320" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="50" windowWidth="19170" windowHeight="7320" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>time/microsecond</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -63,6 +65,124 @@
   </si>
   <si>
     <t>Amp/mv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一阶RC上升过程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>R=10.1k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Ω</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C=18.3nF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>t(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>μ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>s)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V(V)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>升高10%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下降10%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二阶RC上升过程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>R=9.999k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Ω</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C=19.4nF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3阶RC上升过程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>R=10.01k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Ω</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C=16.85nF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rise</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fall</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -74,9 +194,9 @@
     <numFmt numFmtId="176" formatCode="0.0_ "/>
     <numFmt numFmtId="177" formatCode="0.00_ "/>
     <numFmt numFmtId="178" formatCode="0.000_ "/>
-    <numFmt numFmtId="180" formatCode="0_ "/>
+    <numFmt numFmtId="179" formatCode="0_ "/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +211,20 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -115,7 +249,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -128,7 +262,7 @@
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -136,6 +270,9 @@
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -433,9 +570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
@@ -677,7 +812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -878,12 +1013,472 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="11.90625" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>24</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.64</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4">
+        <v>20</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>56</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1.32</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="H5">
+        <v>124</v>
+      </c>
+      <c r="I5" s="2">
+        <v>2.52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>88</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="H6">
+        <v>460</v>
+      </c>
+      <c r="I6" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>100</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2.16</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7">
+        <v>12</v>
+      </c>
+      <c r="I7" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>140</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2.76</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="H8">
+        <v>106</v>
+      </c>
+      <c r="I8" s="2">
+        <v>2.52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9">
+        <v>176</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3.14</v>
+      </c>
+      <c r="G9" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="H9">
+        <v>394</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10">
+        <v>208</v>
+      </c>
+      <c r="B10" s="2">
+        <v>3.44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11">
+        <v>248</v>
+      </c>
+      <c r="B11" s="2">
+        <v>3.76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12">
+        <v>288</v>
+      </c>
+      <c r="B12" s="2">
+        <v>3.98</v>
+      </c>
+      <c r="G12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13">
+        <v>340</v>
+      </c>
+      <c r="B13" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14">
+        <v>412</v>
+      </c>
+      <c r="B14" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15">
+        <v>512</v>
+      </c>
+      <c r="B15" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col min="3" max="3" width="12.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>30</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>40</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>50</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>90</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>130</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>250</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1.7999999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>360</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2.52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>500</v>
+      </c>
+      <c r="B13" s="2">
+        <v>3.16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>1000</v>
+      </c>
+      <c r="B14" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>1650</v>
+      </c>
+      <c r="B15" s="2">
+        <v>4.84</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12:E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>100</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.60000000000000009</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>140</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>180</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>250</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>330</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>450</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1.84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>600</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2.3600000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>810</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2.96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>1110</v>
+      </c>
+      <c r="B13" s="2">
+        <v>3.56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>1550</v>
+      </c>
+      <c r="B14" s="2">
+        <v>4.16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>1930</v>
+      </c>
+      <c r="B15" s="2">
+        <v>4.4800000000000004</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>